<commit_message>
feat: inicio das formulas e validações para criar linha de jogo
</commit_message>
<xml_diff>
--- a/Nova BB01.xlsx
+++ b/Nova BB01.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24332"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Users\Bin\OneDrive\bestbuy86\Planilhas Avançadas\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\João Vitor Gouveia\Documents\Programacao\Repositorios\Bestbuy86\sistema-estoque\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A78DF532-4DDF-4830-9549-A033FDB17E2C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="17835"/>
+    <workbookView xWindow="28680" yWindow="3030" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Plan1" sheetId="1" r:id="rId1"/>
@@ -246,7 +247,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="5">
     <numFmt numFmtId="164" formatCode="[$€-2]\ #,##0.00"/>
     <numFmt numFmtId="165" formatCode="&quot;R$&quot;\ #,##0.00"/>
@@ -696,7 +697,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Imagem 1"/>
+        <xdr:cNvPr id="2" name="Imagem 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -734,7 +741,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Imagem 2"/>
+        <xdr:cNvPr id="3" name="Imagem 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -784,7 +797,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="4" name="Imagem 3"/>
+        <xdr:cNvPr id="4" name="Imagem 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000004000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -834,7 +853,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="5" name="Imagem 4"/>
+        <xdr:cNvPr id="5" name="Imagem 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000005000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -884,7 +909,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="6" name="Imagem 5"/>
+        <xdr:cNvPr id="6" name="Imagem 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000006000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -934,7 +965,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="7" name="Imagem 6"/>
+        <xdr:cNvPr id="7" name="Imagem 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000007000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -984,7 +1021,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="8" name="Imagem 7"/>
+        <xdr:cNvPr id="8" name="Imagem 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000008000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -1034,7 +1077,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="9" name="Imagem 8"/>
+        <xdr:cNvPr id="9" name="Imagem 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000009000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -1079,7 +1128,13 @@
     <xdr:ext cx="247650" cy="238125"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="10" name="Imagem 9"/>
+        <xdr:cNvPr id="10" name="Imagem 9">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000A000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -1124,7 +1179,13 @@
     <xdr:ext cx="247650" cy="241676"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="11" name="Imagem 10"/>
+        <xdr:cNvPr id="11" name="Imagem 10">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000B000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -1169,7 +1230,13 @@
     <xdr:ext cx="247650" cy="229250"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="12" name="Imagem 11"/>
+        <xdr:cNvPr id="12" name="Imagem 11">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000C000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -1214,7 +1281,13 @@
     <xdr:ext cx="247650" cy="238125"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="13" name="Imagem 12"/>
+        <xdr:cNvPr id="13" name="Imagem 12">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000D000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -1259,7 +1332,13 @@
     <xdr:ext cx="247650" cy="241676"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="14" name="Imagem 13"/>
+        <xdr:cNvPr id="14" name="Imagem 13">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000E000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -1304,7 +1383,13 @@
     <xdr:ext cx="247650" cy="229250"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="15" name="Imagem 14"/>
+        <xdr:cNvPr id="15" name="Imagem 14">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000F000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -1604,11 +1689,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A4:AH16"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11:K14"/>
+    <sheetView tabSelected="1" topLeftCell="AB4" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="AG10" sqref="AG10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1889,7 +1974,7 @@
       <c r="N12" s="14"/>
       <c r="O12" s="15"/>
       <c r="P12" s="16">
-        <v>115.85688405797102</v>
+        <v>115.856884057971</v>
       </c>
       <c r="Q12" s="16">
         <v>111.34731769146661</v>
@@ -2316,14 +2401,14 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B1:B1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B1:B1048576" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>"Dup, Revo, Reg"</formula1>
     </dataValidation>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="AF14" r:id="rId1"/>
-    <hyperlink ref="AF11" r:id="rId2"/>
-    <hyperlink ref="AF15" r:id="rId3"/>
+    <hyperlink ref="AF14" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="AF11" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="AF15" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
   </hyperlinks>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId4"/>
@@ -2332,7 +2417,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>